<commit_message>
Looked at answer to save time, will have to come back later after forgot, initial approach was a combination of two solutions and seemed to be right track
</commit_message>
<xml_diff>
--- a/42. Trapping Rain Water/Whiteboards/Solution.xlsx
+++ b/42. Trapping Rain Water/Whiteboards/Solution.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 template\Whiteboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\42. Trapping Rain Water\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DE802-9519-4608-B352-D1C1ED0E8E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBD0145-BBA0-4361-BF89-2494BE96AC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,6 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>Ri</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -45,12 +66,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,9 +92,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -384,18 +414,622 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="A1"/>
+  <dimension ref="F3:AY71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AN65" sqref="AN65:AU71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+      <c r="L3" s="1">
+        <v>4</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1">
+        <v>6</v>
+      </c>
+      <c r="O3" s="1">
+        <v>7</v>
+      </c>
+      <c r="P3" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>9</v>
+      </c>
+      <c r="R3" s="1">
+        <v>10</v>
+      </c>
+      <c r="S3" s="1">
+        <v>11</v>
+      </c>
+      <c r="T3" s="1">
+        <v>12</v>
+      </c>
+      <c r="U3" s="1">
+        <v>13</v>
+      </c>
+      <c r="V3" s="1">
+        <v>14</v>
+      </c>
+      <c r="W3" s="1">
+        <v>15</v>
+      </c>
+      <c r="X3" s="1">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>17</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>6</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>5</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1">
+        <v>2</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>2</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="AJ8" s="2"/>
+    </row>
+    <row r="9" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+    </row>
+    <row r="10" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AN10" s="2"/>
+    </row>
+    <row r="11" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AN11" s="2"/>
+    </row>
+    <row r="12" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AN12" s="2"/>
+    </row>
+    <row r="13" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="2"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AN13" s="2"/>
+    </row>
+    <row r="14" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1">
+        <v>6</v>
+      </c>
+      <c r="L14" s="1">
+        <v>6</v>
+      </c>
+      <c r="M14" s="1">
+        <v>6</v>
+      </c>
+      <c r="N14" s="1">
+        <v>6</v>
+      </c>
+      <c r="O14" s="1">
+        <v>5</v>
+      </c>
+      <c r="P14" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>1</v>
+      </c>
+      <c r="R14" s="1">
+        <v>1</v>
+      </c>
+      <c r="S14" s="1">
+        <v>2</v>
+      </c>
+      <c r="T14" s="1">
+        <v>2</v>
+      </c>
+      <c r="U14" s="1">
+        <v>2</v>
+      </c>
+      <c r="V14" s="1">
+        <v>2</v>
+      </c>
+      <c r="W14" s="1">
+        <v>2</v>
+      </c>
+      <c r="X14" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AN14" s="2"/>
+    </row>
+    <row r="15" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>2</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2</v>
+      </c>
+      <c r="N15" s="1">
+        <v>2</v>
+      </c>
+      <c r="O15" s="1">
+        <v>6</v>
+      </c>
+      <c r="P15" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>8</v>
+      </c>
+      <c r="R15" s="1">
+        <v>9</v>
+      </c>
+      <c r="S15" s="1">
+        <v>10</v>
+      </c>
+      <c r="T15" s="1">
+        <v>10</v>
+      </c>
+      <c r="U15" s="1">
+        <v>12</v>
+      </c>
+      <c r="V15" s="1">
+        <v>12</v>
+      </c>
+      <c r="W15" s="1">
+        <v>12</v>
+      </c>
+      <c r="X15" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="6:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AY16" s="2"/>
+    </row>
+    <row r="17" spans="7:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AX17" s="2"/>
+      <c r="AY17" s="2"/>
+    </row>
+    <row r="18" spans="7:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW18" s="2"/>
+      <c r="AX18" s="2"/>
+      <c r="AY18" s="2"/>
+    </row>
+    <row r="19" spans="7:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA19" s="2"/>
+      <c r="AV19" s="2"/>
+      <c r="AW19" s="2"/>
+      <c r="AX19" s="2"/>
+      <c r="AY19" s="2"/>
+    </row>
+    <row r="20" spans="7:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AU20" s="2"/>
+      <c r="AV20" s="2"/>
+      <c r="AW20" s="2"/>
+      <c r="AX20" s="2"/>
+      <c r="AY20" s="2"/>
+    </row>
+    <row r="21" spans="7:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AT21" s="2"/>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2"/>
+      <c r="AX21" s="2"/>
+      <c r="AY21" s="2"/>
+    </row>
+    <row r="22" spans="7:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+      <c r="AM22" s="2"/>
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="2"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="2"/>
+      <c r="AW22" s="2"/>
+      <c r="AX22" s="2"/>
+      <c r="AY22" s="2"/>
+    </row>
+    <row r="23" spans="7:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AM23" s="2"/>
+    </row>
+    <row r="24" spans="7:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="2"/>
+      <c r="AM24" s="2"/>
+    </row>
+    <row r="25" spans="7:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="2"/>
+      <c r="AM25" s="2"/>
+    </row>
+    <row r="26" spans="7:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG26" s="2"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="2"/>
+      <c r="AM26" s="2"/>
+    </row>
+    <row r="33" spans="24:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z33" s="2"/>
+      <c r="AJ33" s="2"/>
+    </row>
+    <row r="34" spans="24:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+      <c r="AJ34" s="2"/>
+      <c r="AK34" s="2"/>
+    </row>
+    <row r="35" spans="24:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X35" s="2"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="2"/>
+      <c r="AD35" s="2"/>
+      <c r="AJ35" s="2"/>
+      <c r="AK35" s="2"/>
+      <c r="AN35" s="2"/>
+    </row>
+    <row r="36" spans="24:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X36" s="2"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AH36" s="2"/>
+      <c r="AJ36" s="2"/>
+      <c r="AK36" s="2"/>
+      <c r="AN36" s="2"/>
+    </row>
+    <row r="37" spans="24:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X37" s="2"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2"/>
+      <c r="AD37" s="2"/>
+      <c r="AH37" s="2"/>
+      <c r="AJ37" s="2"/>
+      <c r="AK37" s="2"/>
+      <c r="AN37" s="2"/>
+      <c r="AP37" s="2"/>
+    </row>
+    <row r="38" spans="24:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X38" s="2"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AH38" s="2"/>
+      <c r="AJ38" s="2"/>
+      <c r="AK38" s="2"/>
+      <c r="AN38" s="2"/>
+      <c r="AP38" s="2"/>
+    </row>
+    <row r="39" spans="24:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X39" s="2"/>
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AH39" s="2"/>
+      <c r="AJ39" s="2"/>
+      <c r="AK39" s="2"/>
+      <c r="AN39" s="2"/>
+      <c r="AP39" s="2"/>
+    </row>
+    <row r="46" spans="24:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA46" s="2"/>
+    </row>
+    <row r="47" spans="24:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA47" s="2"/>
+      <c r="AB47" s="2"/>
+    </row>
+    <row r="48" spans="24:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z48" s="2"/>
+      <c r="AA48" s="2"/>
+      <c r="AB48" s="2"/>
+    </row>
+    <row r="49" spans="24:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z49" s="2"/>
+      <c r="AA49" s="2"/>
+      <c r="AB49" s="2"/>
+      <c r="AC49" s="2"/>
+    </row>
+    <row r="50" spans="24:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y50" s="2"/>
+      <c r="Z50" s="2"/>
+      <c r="AA50" s="2"/>
+      <c r="AB50" s="2"/>
+      <c r="AC50" s="2"/>
+    </row>
+    <row r="51" spans="24:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y51" s="2"/>
+      <c r="Z51" s="2"/>
+      <c r="AA51" s="2"/>
+      <c r="AB51" s="2"/>
+      <c r="AC51" s="2"/>
+      <c r="AD51" s="2"/>
+    </row>
+    <row r="52" spans="24:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X52" s="2"/>
+      <c r="Y52" s="2"/>
+      <c r="Z52" s="2"/>
+      <c r="AA52" s="2"/>
+      <c r="AB52" s="2"/>
+      <c r="AC52" s="2"/>
+      <c r="AD52" s="2"/>
+    </row>
+    <row r="65" spans="13:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM65" s="2"/>
+    </row>
+    <row r="66" spans="13:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R66" s="2"/>
+      <c r="AC66" s="2"/>
+      <c r="AM66" s="2"/>
+      <c r="AV66" s="2"/>
+    </row>
+    <row r="67" spans="13:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M67" s="2"/>
+      <c r="R67" s="2"/>
+      <c r="AC67" s="2"/>
+      <c r="AM67" s="2"/>
+      <c r="AV67" s="2"/>
+    </row>
+    <row r="68" spans="13:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M68" s="2"/>
+      <c r="R68" s="2"/>
+      <c r="AC68" s="2"/>
+      <c r="AM68" s="2"/>
+      <c r="AV68" s="2"/>
+    </row>
+    <row r="69" spans="13:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M69" s="2"/>
+      <c r="R69" s="2"/>
+      <c r="AC69" s="2"/>
+      <c r="AM69" s="2"/>
+      <c r="AV69" s="2"/>
+    </row>
+    <row r="70" spans="13:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M70" s="2"/>
+      <c r="R70" s="2"/>
+      <c r="AC70" s="2"/>
+      <c r="AM70" s="2"/>
+      <c r="AV70" s="2"/>
+    </row>
+    <row r="71" spans="13:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M71" s="2"/>
+      <c r="R71" s="2"/>
+      <c r="AC71" s="2"/>
+      <c r="AM71" s="2"/>
+      <c r="AV71" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3744B6E-605E-4123-9932-6354F9617CBD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>